<commit_message>
Updated Notes & Ideas
* Added 8 additional refences
</commit_message>
<xml_diff>
--- a/Rocket Specs.xlsx
+++ b/Rocket Specs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Google Drive\Rocket Reference\Git\rr-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan paplaczyk\Google Drive\Rocket Reference\Git\rr-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E783AC-1DDB-4F09-B836-E4F679CC5ECD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE57B926-6979-4B19-9728-9D2B46A5BF0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Launch Vehicles" sheetId="1" r:id="rId1"/>
@@ -20,9 +19,9 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Pap</author>
   </authors>
   <commentList>
-    <comment ref="H51" authorId="0" shapeId="0" xr:uid="{3EFEA1D7-B587-49E5-9D72-0A88DDE80BFD}">
+    <comment ref="H51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +44,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Top of LES</t>
         </r>
@@ -56,12 +55,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Pap</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{09F365D0-416A-446B-8176-0292924FF192}">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,13 +68,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Includes the Interstage</t>
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{12A98E50-BFBF-403D-B49C-C69F62733F45}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Fin Edge to Fin Edge</t>
         </r>
@@ -94,12 +93,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Pap</author>
   </authors>
   <commentList>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{4002218C-C073-4E60-AF24-A6E0F78B0C96}">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,13 +106,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Factor Gimbal Mass to be 0.0007 lb per lbf of thrust from 1972 study NASA-CR-129135 Aerosapce Synthesis Program</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{83B97D9A-6062-4970-A1AC-EDF24ACC6A68}">
+    <comment ref="Q5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -121,13 +120,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Factor Gimbal Mass to be 0.0007 lb per lbf of thrust from 1972 study NASA-CR-129135 Aerosapce Synthesis Program</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{8938443B-9B8C-4970-BE33-75ADBCA2E30B}">
+    <comment ref="Q7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -135,13 +134,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Factor Gimbal Mass to be 0.0007 lb per lbf of thrust from 1972 study NASA-CR-129135 Aerosapce Synthesis Program</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0" shapeId="0" xr:uid="{6D6AE3B7-F28D-4AE3-AC03-FCFD6544E04B}">
+    <comment ref="Q9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +148,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Factor Gimbal Mass to be 0.0007 lb per lbf of thrust from 1972 study NASA-CR-129135 Aerosapce Synthesis Program</t>
         </r>
@@ -160,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="298">
   <si>
     <t>LV</t>
   </si>
@@ -1045,12 +1044,21 @@
   </si>
   <si>
     <t>NASA</t>
+  </si>
+  <si>
+    <t>J-2 200K</t>
+  </si>
+  <si>
+    <t>S-II, S-IVB</t>
+  </si>
+  <si>
+    <t>J-2 225K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1064,7 +1072,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1093,18 +1101,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1112,12 +1144,6 @@
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1153,70 +1179,89 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="PersonalUDF"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="IN2M"/>
+      <definedName name="LB2KG"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{73815901-8414-40EF-AB3D-E7F9387784D7}" name="Table2" displayName="Table2" ref="A1:M180" totalsRowShown="0">
-  <autoFilter ref="A1:M180" xr:uid="{CF3B8BC2-A280-4EF8-89D5-B331496FC368}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M180" totalsRowShown="0">
+  <autoFilter ref="A1:M180">
     <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
+      <colorFilter dxfId="7"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:M180">
     <sortCondition ref="E1:E180"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{46D91DB2-A452-47C4-A419-17B56A70CCB8}" name="LV"/>
-    <tableColumn id="2" xr3:uid="{056E6DBC-4D6F-4D6B-A6DA-1269FA5475B8}" name="Country"/>
-    <tableColumn id="3" xr3:uid="{3D3AA713-A01C-4925-9AC1-1D8C77486821}" name="Family"/>
-    <tableColumn id="13" xr3:uid="{38D52EBA-B6F3-4FF5-ADEC-27FBB6C49F68}" name="Agency"/>
-    <tableColumn id="4" xr3:uid="{4F0C3C58-5A3C-4D5E-9CE0-A635F5DA6276}" name="First Launch" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{85B26A7B-4F5A-4920-BC13-48B3DF190C06}" name="Last Launch" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C84BAB22-5B2E-418A-81C0-52771A64B02F}" name="Orbital Flights"/>
-    <tableColumn id="7" xr3:uid="{FA61331B-B689-4EE6-B1E0-8D9F52731B0D}" name="Height"/>
-    <tableColumn id="8" xr3:uid="{9E051F27-5810-4DF6-B38B-7F34C29A30DE}" name="Dry Mass"/>
-    <tableColumn id="9" xr3:uid="{D291F012-4027-4431-9960-BC528597F433}" name="Liftoff Mass"/>
-    <tableColumn id="10" xr3:uid="{2C6A67EB-739A-403A-B7E3-40384F234A72}" name="Stages"/>
-    <tableColumn id="11" xr3:uid="{020B3A87-58B8-455D-B2BA-936D5B2CAD98}" name="Source"/>
-    <tableColumn id="12" xr3:uid="{5D5BBEA9-6092-40AA-91DC-2C14899A49BD}" name="Launches"/>
+    <tableColumn id="1" name="LV"/>
+    <tableColumn id="2" name="Country"/>
+    <tableColumn id="3" name="Family"/>
+    <tableColumn id="13" name="Agency"/>
+    <tableColumn id="4" name="First Launch" dataDxfId="6"/>
+    <tableColumn id="5" name="Last Launch" dataDxfId="5"/>
+    <tableColumn id="6" name="Orbital Flights"/>
+    <tableColumn id="7" name="Height"/>
+    <tableColumn id="8" name="Dry Mass"/>
+    <tableColumn id="9" name="Liftoff Mass"/>
+    <tableColumn id="10" name="Stages"/>
+    <tableColumn id="11" name="Source"/>
+    <tableColumn id="12" name="Launches"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E8E7155B-DD50-49EF-9783-96A6FF6E0B10}" name="Table1" displayName="Table1" ref="A1:X11" totalsRowShown="0">
-  <autoFilter ref="A1:X11" xr:uid="{C9100D55-8A70-4C51-BFF2-B7467913C5C8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X14" totalsRowShown="0">
+  <autoFilter ref="A1:X14"/>
   <sortState ref="A2:W11">
     <sortCondition ref="V1:V11"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{8B27E4C4-A249-44DF-91F8-4687AC807918}" name="Engine"/>
-    <tableColumn id="2" xr3:uid="{65B30C93-87C4-4677-9D85-74C1E54C7CA5}" name="Stage"/>
-    <tableColumn id="3" xr3:uid="{2AB1FD26-0CA6-48CC-908E-4DDF8C5E5FF7}" name="LV"/>
-    <tableColumn id="4" xr3:uid="{74E49A97-AAC8-416B-AEFC-5CE674012505}" name="Length">
+    <tableColumn id="1" name="Engine"/>
+    <tableColumn id="2" name="Stage"/>
+    <tableColumn id="3" name="LV"/>
+    <tableColumn id="4" name="Length">
       <calculatedColumnFormula>[1]!IN2M(101.61)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{80584F54-066B-4E64-85EA-7EAD4A2DFB16}" name="Diameter">
+    <tableColumn id="5" name="Diameter">
       <calculatedColumnFormula>[1]!IN2M(45.49)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A5D0FADB-D590-4E09-9A23-773BB3EC74F9}" name="Thrust (SL)"/>
-    <tableColumn id="7" xr3:uid="{58BC5EAF-56F9-45F9-884D-41882ADC2D1E}" name="Thrust (Vac)"/>
-    <tableColumn id="8" xr3:uid="{D59CC748-6F69-4313-AA73-C4859C74DB8D}" name="Burn Time"/>
-    <tableColumn id="9" xr3:uid="{542F191B-5F62-4E71-9434-BD73790A0645}" name="ISP (SL)"/>
-    <tableColumn id="10" xr3:uid="{C781136E-0DC2-44A7-B0D1-BA2E3D9695E4}" name="ISP (Vac)"/>
-    <tableColumn id="11" xr3:uid="{43803DB1-46AA-4326-AF6C-7083D1503525}" name="Flow Rate"/>
-    <tableColumn id="12" xr3:uid="{29449D02-9443-4988-9F7E-6320CCBBE68D}" name="Throttle"/>
-    <tableColumn id="13" xr3:uid="{24DA6064-1337-4EC5-9C4D-27C139324CDA}" name="Fuel"/>
-    <tableColumn id="14" xr3:uid="{24A259A3-25C0-4766-9779-07AE7597B503}" name="Oxidizer"/>
-    <tableColumn id="15" xr3:uid="{7BC30D63-97FC-401D-8809-B34EE4855CBB}" name="Mixture Ratio"/>
-    <tableColumn id="16" xr3:uid="{D8843B4C-B4DA-479A-B175-957DA82CB580}" name="Expansion Ratio"/>
-    <tableColumn id="17" xr3:uid="{3C428537-C620-4555-8296-9196FF5F2FD3}" name="Mass"/>
-    <tableColumn id="18" xr3:uid="{AE3B56B4-9216-4B45-9F3F-A59E34A17CE8}" name="Chamber Pressure (psia)"/>
-    <tableColumn id="19" xr3:uid="{A6BF9948-BC0A-4DC6-AFC0-E8CD60D12B38}" name="Gimbal Range"/>
-    <tableColumn id="20" xr3:uid="{05EDBA73-90FD-41FA-A937-C816C901895D}" name="Gimbal Rate"/>
-    <tableColumn id="21" xr3:uid="{DD7824AD-469B-4928-9708-217DF655FC78}" name="Ignition Timing"/>
-    <tableColumn id="22" xr3:uid="{7FB4F309-165F-4479-A165-D095C4A165DB}" name="First Flight"/>
-    <tableColumn id="23" xr3:uid="{256D2CC6-9AD0-4289-9AAA-C71058D33489}" name="Notes"/>
-    <tableColumn id="24" xr3:uid="{CED17D85-4DE2-43B4-BD99-B341969FEFDA}" name="Sources"/>
+    <tableColumn id="6" name="Thrust (SL)"/>
+    <tableColumn id="7" name="Thrust (Vac)"/>
+    <tableColumn id="8" name="Burn Time"/>
+    <tableColumn id="9" name="ISP (SL)"/>
+    <tableColumn id="10" name="ISP (Vac)"/>
+    <tableColumn id="11" name="Flow Rate"/>
+    <tableColumn id="12" name="Throttle"/>
+    <tableColumn id="13" name="Fuel"/>
+    <tableColumn id="14" name="Oxidizer"/>
+    <tableColumn id="15" name="Mixture Ratio"/>
+    <tableColumn id="16" name="Expansion Ratio"/>
+    <tableColumn id="17" name="Mass"/>
+    <tableColumn id="18" name="Chamber Pressure (psia)"/>
+    <tableColumn id="19" name="Gimbal Range"/>
+    <tableColumn id="20" name="Gimbal Rate" dataDxfId="4"/>
+    <tableColumn id="21" name="Ignition Timing" dataDxfId="3"/>
+    <tableColumn id="22" name="First Flight" dataDxfId="2"/>
+    <tableColumn id="23" name="Notes" dataDxfId="1"/>
+    <tableColumn id="24" name="Sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1518,11 +1563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AED7E730-D19C-44A8-86E2-3EA4822F6F6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection sqref="A1:D180"/>
     </sheetView>
   </sheetViews>
@@ -2941,9 +2986,9 @@
       <c r="G59">
         <v>12</v>
       </c>
-      <c r="H59">
-        <f>[1]!FT2M(365)</f>
-        <v>111.25200000000001</v>
+      <c r="H59" t="e">
+        <f ca="1">[1]!FT2M(365)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I59">
         <f>[1]!LB2KG(553000)</f>
@@ -3439,9 +3484,9 @@
       <c r="G80">
         <v>1</v>
       </c>
-      <c r="H80">
-        <f>[1]!FT2M(346)</f>
-        <v>105.46080000000001</v>
+      <c r="H80" t="e">
+        <f ca="1">[1]!FT2M(346)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I80">
         <f>[1]!LB2KG(585000)</f>
@@ -5744,7 +5789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B982B88-E467-4BB2-8BCC-6CD25ED1A980}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -5790,9 +5835,9 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <f>[1]!FT2M(59.1)</f>
-        <v>18.013680000000001</v>
+      <c r="C2" t="e">
+        <f ca="1">[1]!FT2M(59.1)</f>
+        <v>#NAME?</v>
       </c>
       <c r="D2">
         <v>6.61416</v>
@@ -5819,17 +5864,17 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <f>[1]!FT2M(80.2)</f>
-        <v>24.444960000000002</v>
-      </c>
-      <c r="D3">
-        <f>[1]!FT2M(22.8)</f>
-        <v>6.9494400000000009</v>
-      </c>
-      <c r="E3">
-        <f>[1]!FT2M(40.7)</f>
-        <v>12.405360000000002</v>
+      <c r="C3" t="e">
+        <f ca="1">[1]!FT2M(80.2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D3" t="e">
+        <f ca="1">[1]!FT2M(22.8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E3" t="e">
+        <f ca="1">[1]!FT2M(40.7)</f>
+        <v>#NAME?</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -5853,12 +5898,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF43747-4999-4BFF-A8DE-9192B0B803DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5967,11 +6012,11 @@
         <v>23</v>
       </c>
       <c r="D2">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E2">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F2">
@@ -6007,22 +6052,23 @@
         <v>8</v>
       </c>
       <c r="Q2">
-        <f>[1]!LB2KG(2003)</f>
+        <f>[2]!LB2KG(2003)</f>
         <v>908.54477599999996</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>0</v>
       </c>
-      <c r="V2">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4">
         <v>1961</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6037,11 +6083,11 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E3">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F3">
@@ -6077,22 +6123,23 @@
         <v>8</v>
       </c>
       <c r="Q3">
-        <f>[1]!LB2KG(2003+140)</f>
+        <f>[2]!LB2KG(2003+140)</f>
         <v>972.04765599999996</v>
       </c>
       <c r="S3">
         <v>8</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="V3">
+      <c r="U3" s="4"/>
+      <c r="V3" s="4">
         <v>1961</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6107,11 +6154,11 @@
         <v>29</v>
       </c>
       <c r="D4">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E4">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F4">
@@ -6147,22 +6194,23 @@
         <v>8</v>
       </c>
       <c r="Q4">
-        <f>[1]!LB2KG(2003)</f>
+        <f>[2]!LB2KG(2003)</f>
         <v>908.54477599999996</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>0</v>
       </c>
-      <c r="V4">
+      <c r="U4" s="4"/>
+      <c r="V4" s="4">
         <v>1964</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="X4" t="s">
+      <c r="X4" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6177,11 +6225,11 @@
         <v>29</v>
       </c>
       <c r="D5">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E5">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F5">
@@ -6217,22 +6265,23 @@
         <v>8</v>
       </c>
       <c r="Q5">
-        <f>[1]!LB2KG(2003+140)</f>
+        <f>[2]!LB2KG(2003+140)</f>
         <v>972.04765599999996</v>
       </c>
       <c r="S5">
         <v>8</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="V5">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4">
         <v>1964</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="X5" t="s">
+      <c r="X5" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6247,11 +6296,11 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E6">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F6">
@@ -6286,22 +6335,23 @@
         <v>8</v>
       </c>
       <c r="Q6">
-        <f>[1]!LB2KG(2003)</f>
+        <f>[2]!LB2KG(2003)</f>
         <v>908.54477599999996</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="4">
         <v>0</v>
       </c>
-      <c r="V6">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
         <v>1966</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="X6" t="s">
+      <c r="X6" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6316,11 +6366,11 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E7">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F7">
@@ -6355,22 +6405,23 @@
         <v>8</v>
       </c>
       <c r="Q7">
-        <f>[1]!LB2KG(2003+140)</f>
+        <f>[2]!LB2KG(2003+140)</f>
         <v>972.04765599999996</v>
       </c>
       <c r="S7">
         <v>8</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="V7">
+      <c r="U7" s="4"/>
+      <c r="V7" s="4">
         <v>1966</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="X7" t="s">
+      <c r="X7" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6385,11 +6436,11 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E8">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F8">
@@ -6410,7 +6461,7 @@
         <v>292</v>
       </c>
       <c r="K8">
-        <f>[1]!LB2KG(6346.72/8)</f>
+        <f>[2]!LB2KG(6346.72/8)</f>
         <v>359.85267728000002</v>
       </c>
       <c r="L8" t="s">
@@ -6429,7 +6480,7 @@
         <v>8</v>
       </c>
       <c r="Q8">
-        <f>[1]!LB2KG(2003)</f>
+        <f>[2]!LB2KG(2003)</f>
         <v>908.54477599999996</v>
       </c>
       <c r="R8">
@@ -6438,19 +6489,19 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="4">
         <v>0</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="4">
         <v>1973</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="X8" t="s">
+      <c r="X8" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6465,11 +6516,11 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <f>[1]!IN2M(101.61)</f>
+        <f>[2]!IN2M(101.61)</f>
         <v>2.5808939999999998</v>
       </c>
       <c r="E9">
-        <f>[1]!IN2M(45.49)</f>
+        <f>[2]!IN2M(45.49)</f>
         <v>1.155446</v>
       </c>
       <c r="F9">
@@ -6490,7 +6541,7 @@
         <v>292</v>
       </c>
       <c r="K9">
-        <f>[1]!LB2KG(6346.72/8)</f>
+        <f>[2]!LB2KG(6346.72/8)</f>
         <v>359.85267728000002</v>
       </c>
       <c r="L9" t="s">
@@ -6509,7 +6560,7 @@
         <v>8</v>
       </c>
       <c r="Q9">
-        <f>[1]!LB2KG(2003+140)</f>
+        <f>[2]!LB2KG(2003+140)</f>
         <v>972.04765599999996</v>
       </c>
       <c r="R9">
@@ -6518,19 +6569,19 @@
       <c r="S9">
         <v>8</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="4">
         <v>1973</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="X9" t="s">
+      <c r="X9" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6545,11 +6596,11 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <f>[1]!IN2M(133)</f>
+        <f>[2]!IN2M(133)</f>
         <v>3.3781999999999996</v>
       </c>
       <c r="E10">
-        <f>[1]!IN2M(80.75)</f>
+        <f>[2]!IN2M(80.75)</f>
         <v>2.05105</v>
       </c>
       <c r="F10">
@@ -6561,7 +6612,7 @@
         <v>1000.8495</v>
       </c>
       <c r="H10">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I10">
         <v>293.81</v>
@@ -6579,10 +6630,10 @@
         <v>5.5</v>
       </c>
       <c r="P10">
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="Q10">
-        <f>[1]!LB2KG(3665)</f>
+        <f>[2]!LB2KG(3665)</f>
         <v>1662.4146800000001</v>
       </c>
       <c r="R10">
@@ -6591,13 +6642,15 @@
       <c r="S10">
         <v>7</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="X10" t="s">
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6612,11 +6665,11 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <f>[1]!IN2M(133)</f>
+        <f>[2]!IN2M(133)</f>
         <v>3.3781999999999996</v>
       </c>
       <c r="E11">
-        <f>[1]!IN2M(80.75)</f>
+        <f>[2]!IN2M(80.75)</f>
         <v>2.05105</v>
       </c>
       <c r="F11">
@@ -6628,7 +6681,7 @@
         <v>867.40290000000005</v>
       </c>
       <c r="H11">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I11">
         <v>293.81</v>
@@ -6646,10 +6699,10 @@
         <v>4.8</v>
       </c>
       <c r="P11">
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="Q11">
-        <f>[1]!LB2KG(3665)</f>
+        <f>[2]!LB2KG(3665)</f>
         <v>1662.4146800000001</v>
       </c>
       <c r="R11">
@@ -6658,15 +6711,184 @@
       <c r="S11">
         <v>7</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="X11" t="s">
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3.3782000000000001</v>
+      </c>
+      <c r="E12">
+        <v>2.05105</v>
+      </c>
+      <c r="G12">
+        <f>[1]!LBF2KN(200000)</f>
+        <v>889.64400000000001</v>
+      </c>
+      <c r="H12">
+        <v>500</v>
+      </c>
+      <c r="J12">
+        <v>418</v>
+      </c>
+      <c r="L12">
+        <v>0.77</v>
+      </c>
+      <c r="M12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <v>27.5</v>
+      </c>
+      <c r="Q12">
+        <f>[1]!LB2KG(3609)</f>
+        <v>1637.013528</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>3.3782000000000001</v>
+      </c>
+      <c r="E13">
+        <v>2.05105</v>
+      </c>
+      <c r="G13">
+        <f>[1]!LBF2KN(225000)</f>
+        <v>1000.8495</v>
+      </c>
+      <c r="H13">
+        <v>500</v>
+      </c>
+      <c r="J13">
+        <v>419</v>
+      </c>
+      <c r="L13">
+        <v>0.77</v>
+      </c>
+      <c r="M13" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13">
+        <v>5.5</v>
+      </c>
+      <c r="P13">
+        <v>27.5</v>
+      </c>
+      <c r="Q13">
+        <f>[1]!LB2KG(3609)</f>
+        <v>1637.013528</v>
+      </c>
+      <c r="S13">
+        <v>7</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>3.3782000000000001</v>
+      </c>
+      <c r="E14">
+        <v>2.05105</v>
+      </c>
+      <c r="G14">
+        <f>[1]!LBF2KN(230000)</f>
+        <v>1023.0906</v>
+      </c>
+      <c r="H14">
+        <v>500</v>
+      </c>
+      <c r="J14">
+        <v>421</v>
+      </c>
+      <c r="L14">
+        <v>0.77</v>
+      </c>
+      <c r="M14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N14" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14">
+        <v>5.5</v>
+      </c>
+      <c r="P14">
+        <v>27.5</v>
+      </c>
+      <c r="Q14">
+        <f>[1]!LB2KG(3621)</f>
+        <v>1642.4566319999999</v>
+      </c>
+      <c r="S14">
+        <v>7</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6678,7 +6900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C6FCA2-FBFE-437C-BBEF-A2487BF7FDD1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -6727,24 +6949,24 @@
       <c r="C2">
         <v>2.016</v>
       </c>
-      <c r="D2">
-        <f>[1]!F2C(-435)</f>
-        <v>-259.44444444444446</v>
-      </c>
-      <c r="E2">
-        <f>[1]!F2C(-422.9)</f>
-        <v>-252.7222222222222</v>
-      </c>
-      <c r="F2">
-        <f>[1]!F2C(399.96)</f>
-        <v>204.42222222222222</v>
+      <c r="D2" t="e">
+        <f ca="1">[1]!F2C(-435)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E2" t="e">
+        <f ca="1">[1]!F2C(-422.9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F2" t="e">
+        <f ca="1">[1]!F2C(399.96)</f>
+        <v>#NAME?</v>
       </c>
       <c r="G2">
         <v>-188.16</v>
       </c>
-      <c r="H2">
-        <f>[1]!LBG2KGL(0.594)</f>
-        <v>7.1176643999999997E-2</v>
+      <c r="H2" t="e">
+        <f ca="1">[1]!LBG2KGL(0.594)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I2" t="s">
         <v>97</v>
@@ -6766,24 +6988,24 @@
       <c r="C3">
         <v>92.016000000000005</v>
       </c>
-      <c r="D3">
-        <f>[1]!F2C(11.84)</f>
-        <v>-11.2</v>
-      </c>
-      <c r="E3">
-        <f>[1]!F2C(70.07)</f>
-        <v>21.149999999999995</v>
-      </c>
-      <c r="F3">
-        <f>[1]!F2C(316.8)</f>
-        <v>158.22222222222223</v>
+      <c r="D3" t="e">
+        <f ca="1">[1]!F2C(11.84)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E3" t="e">
+        <f ca="1">[1]!F2C(70.07)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F3" t="e">
+        <f ca="1">[1]!F2C(316.8)</f>
+        <v>#NAME?</v>
       </c>
       <c r="G3">
         <v>1469</v>
       </c>
-      <c r="H3">
-        <f>[1]!LBG2KGL(11.94)</f>
-        <v>1.43072244</v>
+      <c r="H3" t="e">
+        <f ca="1">[1]!LBG2KGL(11.94)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I3" t="s">
         <v>92</v>
@@ -6811,24 +7033,24 @@
       <c r="C4">
         <v>46.075000000000003</v>
       </c>
-      <c r="D4">
-        <f>[1]!F2C(-62.5)</f>
-        <v>-52.5</v>
-      </c>
-      <c r="E4">
-        <f>[1]!F2C(192.5)</f>
-        <v>89.166666666666671</v>
-      </c>
-      <c r="F4">
-        <f>[1]!F2C(593.6)</f>
-        <v>312</v>
+      <c r="D4" t="e">
+        <f ca="1">[1]!F2C(-62.5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E4" t="e">
+        <f ca="1">[1]!F2C(192.5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F4" t="e">
+        <f ca="1">[1]!F2C(593.6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="G4">
         <v>1195.0999999999999</v>
       </c>
-      <c r="H4">
-        <f>[1]!LBG2KGL(7.29)</f>
-        <v>0.87353154</v>
+      <c r="H4" t="e">
+        <f ca="1">[1]!LBG2KGL(7.29)</f>
+        <v>#NAME?</v>
       </c>
       <c r="I4" t="s">
         <v>85</v>

</xml_diff>